<commit_message>
Update test results data - 2025-24-11 07:23 AM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/IBA Mock/Mock 1.xlsx
+++ b/Results/IBA Mock/Mock 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\IBA Mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F881116-1BAF-4C57-B427-8327023314DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F02F53-4E3B-45AA-8458-FC6995EA7E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,6 +568,7 @@
       <b/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1139,7 +1140,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1249,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I19" si="2">G2*1 + H2*($Z$6)</f>
+        <f t="shared" ref="I2:I25" si="2">G2*1 + H2*($Z$6)</f>
         <v>6.75</v>
       </c>
       <c r="J2">
@@ -1840,7 +1841,7 @@
       </c>
       <c r="Q10">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R10" s="12"/>
       <c r="S10" s="13"/>
@@ -1852,7 +1853,7 @@
       </c>
       <c r="W10">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -2407,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20:I31" si="13">G20*1 + H20*(T24)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J20">
@@ -2415,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M31" si="14">K20*1 + L20*(-0.25)</f>
+        <f t="shared" ref="M20:M31" si="13">K20*1 + L20*(-0.25)</f>
         <v>0</v>
       </c>
       <c r="N20">
@@ -2475,12 +2476,12 @@
         <v>3</v>
       </c>
       <c r="I21">
-        <f t="shared" si="13"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2.25</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -2489,7 +2490,7 @@
         <v>4</v>
       </c>
       <c r="M21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="N21">
@@ -2498,11 +2499,11 @@
       </c>
       <c r="O21">
         <f t="shared" si="6"/>
-        <v>12.5</v>
+        <v>11.75</v>
       </c>
       <c r="P21">
         <f t="shared" si="7"/>
-        <v>17.857142857142858</v>
+        <v>16.785714285714285</v>
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
@@ -2514,7 +2515,7 @@
       <c r="U21" s="11"/>
       <c r="V21">
         <f t="shared" si="11"/>
-        <v>12.5</v>
+        <v>11.75</v>
       </c>
       <c r="W21">
         <f t="shared" si="10"/>
@@ -2549,12 +2550,12 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <f t="shared" si="13"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5.75</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -2563,7 +2564,7 @@
         <v>1</v>
       </c>
       <c r="M22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-0.25</v>
       </c>
       <c r="N22">
@@ -2572,11 +2573,11 @@
       </c>
       <c r="O22">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="P22">
         <f t="shared" si="7"/>
-        <v>11.428571428571429</v>
+        <v>11.071428571428571</v>
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
@@ -2588,7 +2589,7 @@
       <c r="U22" s="11"/>
       <c r="V22">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
@@ -2623,12 +2624,12 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>-2</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2637,7 +2638,7 @@
         <v>4</v>
       </c>
       <c r="M23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N23">
@@ -2646,11 +2647,11 @@
       </c>
       <c r="O23">
         <f t="shared" si="6"/>
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="P23">
         <f t="shared" si="7"/>
-        <v>10.714285714285714</v>
+        <v>7.8571428571428568</v>
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
@@ -2662,7 +2663,7 @@
       <c r="U23" s="11"/>
       <c r="V23">
         <f t="shared" si="11"/>
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="W23">
         <f t="shared" si="10"/>
@@ -2697,12 +2698,12 @@
         <v>4</v>
       </c>
       <c r="I24">
-        <f t="shared" si="13"/>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K24">
         <v>3</v>
@@ -2711,7 +2712,7 @@
         <v>6</v>
       </c>
       <c r="M24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
       <c r="N24">
@@ -2720,11 +2721,11 @@
       </c>
       <c r="O24">
         <f t="shared" si="6"/>
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="P24">
         <f t="shared" si="7"/>
-        <v>33.571428571428569</v>
+        <v>32.142857142857146</v>
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
@@ -2736,7 +2737,7 @@
       <c r="U24" s="11"/>
       <c r="V24">
         <f t="shared" si="11"/>
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
@@ -2771,12 +2772,12 @@
         <v>2</v>
       </c>
       <c r="I25">
-        <f t="shared" si="13"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>3.5</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -2785,7 +2786,7 @@
         <v>3</v>
       </c>
       <c r="M25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.25</v>
       </c>
       <c r="N25">
@@ -2794,11 +2795,11 @@
       </c>
       <c r="O25">
         <f t="shared" si="6"/>
-        <v>16.5</v>
+        <v>16</v>
       </c>
       <c r="P25">
         <f t="shared" si="7"/>
-        <v>23.571428571428569</v>
+        <v>22.857142857142858</v>
       </c>
       <c r="Q25">
         <f t="shared" si="8"/>
@@ -2810,7 +2811,7 @@
       <c r="U25" s="11"/>
       <c r="V25">
         <f t="shared" si="11"/>
-        <v>16.5</v>
+        <v>16</v>
       </c>
       <c r="W25">
         <f t="shared" si="10"/>
@@ -2827,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="I20:I31" si="14">G26*1 + H26*(T30)</f>
         <v>0</v>
       </c>
       <c r="J26">
@@ -2835,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N26">
@@ -2877,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J27">
@@ -2885,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N27">
@@ -2927,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J28">
@@ -2935,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N28">
@@ -2977,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J29">
@@ -2985,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N29">
@@ -3027,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J30">
@@ -3035,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N30">
@@ -3077,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J31">
@@ -3085,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N31">

</xml_diff>

<commit_message>
Update test results data - 2025-28-11 12:46 AM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/IBA Mock/Mock 1.xlsx
+++ b/Results/IBA Mock/Mock 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\IBA Mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F02F53-4E3B-45AA-8458-FC6995EA7E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8FC1E6-C3B7-4EA6-9C54-7219E91E7D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,7 +571,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,8 +614,14 @@
         <bgColor rgb="FF90EE90"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -743,11 +749,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -802,6 +838,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,7 +1185,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1283,13 +1328,15 @@
         <f t="shared" ref="Q2:Q31" si="8">_xlfn.RANK.EQ(P2, $P$2:$P$1000, 0)</f>
         <v>2</v>
       </c>
-      <c r="R2" s="10"/>
+      <c r="R2" s="19">
+        <v>18</v>
+      </c>
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2">
         <f t="shared" ref="V2:V11" si="9">O2+R2+S2+T2+U2</f>
-        <v>17.5</v>
+        <v>35.5</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W31" si="10">_xlfn.RANK.EQ(V2, $V$2:$V$1000, 0)</f>
@@ -1363,17 +1410,19 @@
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="R3" s="10"/>
+      <c r="R3" s="20">
+        <v>9</v>
+      </c>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="W3">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X3" t="s">
         <v>27</v>
@@ -1443,17 +1492,19 @@
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="R4" s="10"/>
+      <c r="R4" s="20">
+        <v>10</v>
+      </c>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
       <c r="V4">
         <f t="shared" si="9"/>
-        <v>-0.5</v>
+        <v>9.5</v>
       </c>
       <c r="W4">
         <f t="shared" si="10"/>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="Y4">
         <f>SUM(Y1:Y3)</f>
@@ -1521,13 +1572,15 @@
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="R5" s="10"/>
+      <c r="R5" s="20">
+        <v>12</v>
+      </c>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
       <c r="V5">
         <f t="shared" si="9"/>
-        <v>8.5</v>
+        <v>20.5</v>
       </c>
       <c r="W5">
         <f t="shared" si="10"/>
@@ -1577,7 +1630,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R6" s="10"/>
+      <c r="R6" s="21"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
@@ -1587,7 +1640,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Y6" t="s">
         <v>31</v>
@@ -1639,7 +1692,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R7" s="10"/>
+      <c r="R7" s="21"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
@@ -1649,7 +1702,7 @@
       </c>
       <c r="W7">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1695,7 +1748,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R8" s="12"/>
+      <c r="R8" s="21"/>
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
@@ -1705,7 +1758,7 @@
       </c>
       <c r="W8">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1769,13 +1822,15 @@
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="R9" s="10"/>
+      <c r="R9" s="20">
+        <v>10</v>
+      </c>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
       <c r="U9" s="11"/>
       <c r="V9">
         <f t="shared" si="9"/>
-        <v>4.25</v>
+        <v>14.25</v>
       </c>
       <c r="W9">
         <f t="shared" si="10"/>
@@ -1843,17 +1898,19 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="R10" s="12"/>
+      <c r="R10" s="20">
+        <v>11.5</v>
+      </c>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
       <c r="V10">
         <f t="shared" si="9"/>
-        <v>11.75</v>
+        <v>23.25</v>
       </c>
       <c r="W10">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1899,7 +1956,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="R11" s="21"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
       <c r="U11" s="11"/>
@@ -1909,7 +1966,7 @@
       </c>
       <c r="W11">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -1955,13 +2012,13 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R12" s="12"/>
+      <c r="R12" s="21"/>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -2007,7 +2064,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R13" s="12"/>
+      <c r="R13" s="21"/>
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
@@ -2017,7 +2074,7 @@
       </c>
       <c r="W13">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -2063,7 +2120,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R14" s="12"/>
+      <c r="R14" s="21"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
@@ -2073,7 +2130,7 @@
       </c>
       <c r="W14">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -2119,7 +2176,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R15" s="10"/>
+      <c r="R15" s="21"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
@@ -2129,7 +2186,7 @@
       </c>
       <c r="W15">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" thickBot="1">
@@ -2175,7 +2232,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R16" s="10"/>
+      <c r="R16" s="21"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
@@ -2185,7 +2242,7 @@
       </c>
       <c r="W16">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2231,7 +2288,7 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R17" s="10"/>
+      <c r="R17" s="21"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
@@ -2241,7 +2298,7 @@
       </c>
       <c r="W17">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2305,13 +2362,15 @@
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="R18" s="12"/>
+      <c r="R18" s="20">
+        <v>11</v>
+      </c>
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
       <c r="V18">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="W18">
         <f t="shared" si="10"/>
@@ -2379,17 +2438,19 @@
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="R19" s="10"/>
+      <c r="R19" s="20">
+        <v>12.5</v>
+      </c>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
       <c r="V19">
         <f t="shared" si="11"/>
-        <v>2.25</v>
+        <v>14.75</v>
       </c>
       <c r="W19">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2435,17 +2496,19 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="R20" s="11"/>
+      <c r="R20" s="20">
+        <v>7.5</v>
+      </c>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
       <c r="V20">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="W20">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2509,17 +2572,19 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="R21" s="11"/>
+      <c r="R21" s="20">
+        <v>20</v>
+      </c>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
       <c r="U21" s="11"/>
       <c r="V21">
         <f t="shared" si="11"/>
-        <v>11.75</v>
+        <v>31.75</v>
       </c>
       <c r="W21">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="28.2" customHeight="1" thickBot="1">
@@ -2583,17 +2648,19 @@
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="R22" s="10"/>
+      <c r="R22" s="20">
+        <v>11.5</v>
+      </c>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
       <c r="V22">
         <f t="shared" si="11"/>
-        <v>7.75</v>
+        <v>19.25</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="43.8" customHeight="1" thickBot="1">
@@ -2657,17 +2724,19 @@
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="R23" s="10"/>
+      <c r="R23" s="20">
+        <v>14.5</v>
+      </c>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
       <c r="U23" s="11"/>
       <c r="V23">
         <f t="shared" si="11"/>
-        <v>5.5</v>
+        <v>20</v>
       </c>
       <c r="W23">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="29.4" customHeight="1" thickBot="1">
@@ -2731,13 +2800,15 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="R24" s="10"/>
+      <c r="R24" s="20">
+        <v>14</v>
+      </c>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
       <c r="V24">
         <f t="shared" si="11"/>
-        <v>22.5</v>
+        <v>36.5</v>
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
@@ -2805,17 +2876,19 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="R25" s="10"/>
+      <c r="R25" s="20">
+        <v>15.5</v>
+      </c>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
       <c r="V25">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>31.5</v>
       </c>
       <c r="W25">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2828,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I20:I31" si="14">G26*1 + H26*(T30)</f>
+        <f t="shared" ref="I26:I31" si="14">G26*1 + H26*(T30)</f>
         <v>0</v>
       </c>
       <c r="J26">
@@ -2865,7 +2938,7 @@
       </c>
       <c r="W26">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2915,7 +2988,7 @@
       </c>
       <c r="W27">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -2965,7 +3038,7 @@
       </c>
       <c r="W28">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -3015,7 +3088,7 @@
       </c>
       <c r="W29">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -3065,7 +3138,7 @@
       </c>
       <c r="W30">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1">
@@ -3115,7 +3188,7 @@
       </c>
       <c r="W31">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>